<commit_message>
add datas and logics
</commit_message>
<xml_diff>
--- a/Jumlah Kasus Kejahatan Pembunuhan Pada Satu Tahun Terakhir.xlsx
+++ b/Jumlah Kasus Kejahatan Pembunuhan Pada Satu Tahun Terakhir.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosral/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosral/Desktop/tetris/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B83CFF-62C6-D843-8E0B-E81E341FD3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6E50F8-2645-3545-80D3-3D0462619400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,107 +471,107 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="19.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:B11" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>